<commit_message>
correção preço e moeda
</commit_message>
<xml_diff>
--- a/Scrap/Dados.xlsx
+++ b/Scrap/Dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnova\.gitRepositories\Scrap\Scrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB386E2-B8E9-4D55-B4BC-471625218D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A33932B-2B73-4EDA-A608-715A3E9C39A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{7DBB027D-C5BD-40A7-8659-AB2808C8076E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>HorarioPartida</t>
   </si>
@@ -79,9 +79,6 @@
     <t>qua., 15/11</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>8:55</t>
   </si>
   <si>
@@ -107,6 +104,18 @@
   </si>
   <si>
     <t>10 h 45 min.</t>
+  </si>
+  <si>
+    <t>72.091</t>
+  </si>
+  <si>
+    <t>pontos</t>
+  </si>
+  <si>
+    <t>98.876</t>
+  </si>
+  <si>
+    <t>80.105</t>
   </si>
 </sst>
 </file>
@@ -475,7 +484,7 @@
     <col min="5" max="5" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -509,18 +518,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
@@ -532,10 +541,10 @@
         <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -543,42 +552,42 @@
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -590,10 +599,10 @@
         <v>13</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -601,28 +610,28 @@
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>